<commit_message>
bank live project day 4 done
</commit_message>
<xml_diff>
--- a/DemoBankRealTimeProject/out/production/DemoBankRealTimeProject/resources/parameters.xlsx
+++ b/DemoBankRealTimeProject/out/production/DemoBankRealTimeProject/resources/parameters.xlsx
@@ -16,13 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>mngr215270</t>
   </si>
@@ -31,6 +25,27 @@
   </si>
   <si>
     <t>xxx</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Valid userId &amp; password</t>
+  </si>
+  <si>
+    <t>Invalid userId &amp; valid password</t>
+  </si>
+  <si>
+    <t>Invalid userId &amp; invalid password</t>
+  </si>
+  <si>
+    <t>Valid userId &amp; invalid password</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -406,52 +421,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="C3" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
+      <c r="C5" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>